<commit_message>
Evaluation of RF with BERT embedded questions
</commit_message>
<xml_diff>
--- a/Notebooks/df_metrics_scores.xlsx
+++ b/Notebooks/df_metrics_scores.xlsx
@@ -468,10 +468,10 @@
         <v>0.3418353931107021</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2224121307739504</v>
+        <v>0.2265316855114383</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5891839861869812</v>
+        <v>0.4815058410167694</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
         <v>0.2878266035171254</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6166982715371426</v>
+        <v>0.6166891672684198</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5704609227980255</v>
+        <v>0.5721471350418985</v>
       </c>
       <c r="E3" t="n">
-        <v>0.643469512462616</v>
+        <v>0.5200661420822144</v>
       </c>
     </row>
     <row r="4">
@@ -506,10 +506,10 @@
         <v>0.4873263182373118</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7342596360676705</v>
+        <v>0.7333003895122376</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5509036779403687</v>
+        <v>0.4010415077209473</v>
       </c>
     </row>
     <row r="5">
@@ -522,13 +522,13 @@
         <v>0.1610929649574388</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7446057741365187</v>
+        <v>0.7445664032668693</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5245024400786253</v>
+        <v>0.5295127493052906</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7799243927001953</v>
+        <v>0.7511604428291321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>